<commit_message>
tests updated and went through
</commit_message>
<xml_diff>
--- a/tests/behavior/input/BehaviorScenario_Household.xlsx
+++ b/tests/behavior/input/BehaviorScenario_Household.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX_temp/projects/linda/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/FLEX/tests/behavior/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5304EE07-5903-1A46-BB5C-E25CD2AD5AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15DF89F-A2E6-AF45-9E92-533DD270A872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14680" yWindow="-17220" windowWidth="21400" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="1840" windowWidth="21640" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="no_teleworking" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="7">
   <si>
     <t>value</t>
   </si>
@@ -61,9 +61,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -117,10 +124,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -574,8 +582,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E4ED849-4093-0F4D-BA60-1A2F7F091CAB}" name="Table132" displayName="Table132" ref="A1:F11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:F11" xr:uid="{6E4ED849-4093-0F4D-BA60-1A2F7F091CAB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E4ED849-4093-0F4D-BA60-1A2F7F091CAB}" name="Table132" displayName="Table132" ref="A1:F9" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:F9" xr:uid="{6E4ED849-4093-0F4D-BA60-1A2F7F091CAB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7B90C219-5ADF-D64C-93ED-97F77646ED90}" name="id_household_type" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{7C0DE424-755F-4549-93F8-FC07A6BE7A90}" name="id_household_composition_type" dataDxfId="20"/>
@@ -915,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5762E8D-4362-3546-8827-C3ED2CB2B6E8}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -970,31 +978,31 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4">
-        <v>2</v>
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -1010,142 +1018,102 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2</v>
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4">
-        <v>3</v>
+      <c r="B9" s="5">
+        <v>2</v>
       </c>
       <c r="C9" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1648,6 +1616,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed526690-1b82-4476-9598-c0eeafad58f9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001383FD7952F44C4AA66F138C1496F932" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0f10bb0856646bfda2b94dc29ed0a887">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed526690-1b82-4476-9598-c0eeafad58f9" xmlns:ns3="f971c2dd-4979-4752-97a1-eb062e2c22bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca21336e7eb6462c50ac4645cdd355ca" ns2:_="" ns3:_="">
     <xsd:import namespace="ed526690-1b82-4476-9598-c0eeafad58f9"/>
@@ -1852,27 +1840,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE03864-EF8F-45D0-B8AF-9F190340F3F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f971c2dd-4979-4752-97a1-eb062e2c22bf"/>
+    <ds:schemaRef ds:uri="ed526690-1b82-4476-9598-c0eeafad58f9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed526690-1b82-4476-9598-c0eeafad58f9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C498-74B4-4650-B402-97A5D02496A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8831E31-2A91-4E0B-B823-0BFA5718552C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1889,23 +1876,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C498-74B4-4650-B402-97A5D02496A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE03864-EF8F-45D0-B8AF-9F190340F3F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f971c2dd-4979-4752-97a1-eb062e2c22bf"/>
-    <ds:schemaRef ds:uri="ed526690-1b82-4476-9598-c0eeafad58f9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>